<commit_message>
feature/GDE-7585 script and data set updates for RPA Scenario 2 primaries
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S2_EU_RPA_ExternallDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S2_EU_RPA_ExternallDeal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\EU_Entity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81467DCD-489D-4E5D-B19E-F3BD5075BAA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F0763-FB3B-4D7B-888E-A551E86C31D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -2987,7 +2987,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3051,6 +3051,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3131,7 +3137,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3278,6 +3284,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10026,11 +10034,11 @@
   </sheetPr>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
+      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10329,9 +10337,9 @@
   </sheetPr>
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10507,10 +10515,10 @@
       <c r="Q2" s="93" t="s">
         <v>545</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="104" t="s">
         <v>368</v>
       </c>
       <c r="T2" s="93" t="s">
@@ -10522,7 +10530,7 @@
       <c r="W2" s="93" t="s">
         <v>545</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="105" t="s">
         <v>597</v>
       </c>
       <c r="Y2" s="93" t="s">
@@ -10593,10 +10601,10 @@
       <c r="Q3" s="93" t="s">
         <v>545</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="104" t="s">
         <v>368</v>
       </c>
       <c r="T3" s="93" t="s">
@@ -10608,7 +10616,7 @@
       <c r="W3" s="93" t="s">
         <v>545</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="X3" s="105" t="s">
         <v>597</v>
       </c>
       <c r="Y3" s="93" t="s">
@@ -10679,10 +10687,10 @@
       <c r="Q4" s="93" t="s">
         <v>545</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="104" t="s">
         <v>368</v>
       </c>
       <c r="T4" s="93" t="s">
@@ -10694,7 +10702,7 @@
       <c r="W4" s="93" t="s">
         <v>545</v>
       </c>
-      <c r="X4" s="14" t="s">
+      <c r="X4" s="105" t="s">
         <v>597</v>
       </c>
       <c r="Y4" s="93" t="s">

</xml_diff>

<commit_message>
feature/GDE-7587 script and data set updates for charge upfront fee for RPA Scenario 2
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S2_EU_RPA_ExternallDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S2_EU_RPA_ExternallDeal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\EU_Entity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F0763-FB3B-4D7B-888E-A551E86C31D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090CD4D6-3034-42FA-86F5-D588253A9E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="929">
   <si>
     <t>rowid</t>
   </si>
@@ -1597,13 +1597,13 @@
     <t>R2_</t>
   </si>
   <si>
-    <t>RPA EXTERNAL 100M EURO27102020180941RUQ</t>
-  </si>
-  <si>
-    <t>R2_27102020180943KEK</t>
-  </si>
-  <si>
-    <t>INTFULDRAW27102020183553MRA</t>
+    <t>RPA EXTERNAL 100M EURO28102020152508YAI</t>
+  </si>
+  <si>
+    <t>R2_28102020152511XVO</t>
+  </si>
+  <si>
+    <t>INTFULDRAW28102020153405IIQ</t>
   </si>
   <si>
     <t>Sales Group 1</t>
@@ -1648,7 +1648,7 @@
     <t>1.00000000000</t>
   </si>
   <si>
-    <t>02-Jul-2020</t>
+    <t>06-Jul-2020</t>
   </si>
   <si>
     <t>Euro LIBOR Option</t>
@@ -1705,7 +1705,7 @@
     <t>5,000</t>
   </si>
   <si>
-    <t>PARDRAW27102020184602AJM</t>
+    <t>PARDRAW28102020154312DBX</t>
   </si>
   <si>
     <t>27-May-2020</t>
@@ -1714,7 +1714,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>INTUND27102020185600UZT</t>
+    <t>INTUND28102020155226KLJ</t>
   </si>
   <si>
     <t>UpfrontFee_CategoryType</t>
@@ -1969,7 +1969,7 @@
     <t>50,000,000.00</t>
   </si>
   <si>
-    <t>01-Jul-2025</t>
+    <t>07-Jul-2025</t>
   </si>
   <si>
     <t>Loan</t>
@@ -2080,148 +2080,148 @@
     <t>2.5</t>
   </si>
   <si>
+    <t>LIBOR</t>
+  </si>
+  <si>
+    <t>Fixed Rate Option</t>
+  </si>
+  <si>
+    <t>Facility B Partially Drawn</t>
+  </si>
+  <si>
+    <t>Facility Internal Undrawn</t>
+  </si>
+  <si>
+    <t>Primary_Lender</t>
+  </si>
+  <si>
+    <t>Primary_LenderLoc</t>
+  </si>
+  <si>
+    <t>Primary_RiskBook</t>
+  </si>
+  <si>
+    <t>Primary_PctOfDeal</t>
+  </si>
+  <si>
+    <t>BuySellPrice</t>
+  </si>
+  <si>
+    <t>SellAmount</t>
+  </si>
+  <si>
+    <t>Primary_Contact</t>
+  </si>
+  <si>
+    <t>Primary_Portfolio</t>
+  </si>
+  <si>
+    <t>Primary_PortfolioBranch</t>
+  </si>
+  <si>
+    <t>Structured Asset Finance</t>
+  </si>
+  <si>
+    <t>02-Jun-2020</t>
+  </si>
+  <si>
+    <t>Facility_Spread</t>
+  </si>
+  <si>
+    <t>Facility_CurrentAvailToDraw</t>
+  </si>
+  <si>
+    <t>Facility_CurrentGlobalOutstandings</t>
+  </si>
+  <si>
+    <t>Outstanding_Type</t>
+  </si>
+  <si>
+    <t>Loan_FacilityName</t>
+  </si>
+  <si>
+    <t>Loan_Alias</t>
+  </si>
+  <si>
+    <t>Loan_PricingOption</t>
+  </si>
+  <si>
+    <t>Loan_RequestedAmount</t>
+  </si>
+  <si>
+    <t>HostBankSharePct</t>
+  </si>
+  <si>
+    <t>Loan_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Loan_MaturityDate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingFrequency</t>
+  </si>
+  <si>
+    <t>Loan_IntCycleFrequency</t>
+  </si>
+  <si>
+    <t>Loan_Accrue</t>
+  </si>
+  <si>
+    <t>Borrower_BaseRate</t>
+  </si>
+  <si>
+    <t>Repayment_ScheduleFrequency</t>
+  </si>
+  <si>
+    <t>Repayment_NumberOfCycles</t>
+  </si>
+  <si>
+    <t>Repayment_TriggerDate</t>
+  </si>
+  <si>
+    <t>Repayment_NonBusDayRule</t>
+  </si>
+  <si>
+    <t>WIP_TransactionType</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingApprovalStatus</t>
+  </si>
+  <si>
+    <t>WIP_OutstandingType</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingRateApprovalStatus</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingReleaseCashflowsStatus</t>
+  </si>
+  <si>
+    <t>Borrower_Profile</t>
+  </si>
+  <si>
+    <t>Remittance_Status</t>
+  </si>
+  <si>
+    <t>Loan_Currency</t>
+  </si>
+  <si>
+    <t>HostBank_GLAccount</t>
+  </si>
+  <si>
+    <t>Borrower_GLAccount</t>
+  </si>
+  <si>
+    <t>Host_Bank</t>
+  </si>
+  <si>
+    <t>NoticeStatus</t>
+  </si>
+  <si>
+    <t>BranchCode</t>
+  </si>
+  <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>LIBOR</t>
-  </si>
-  <si>
-    <t>Fixed Rate Option</t>
-  </si>
-  <si>
-    <t>Facility B Partially Drawn</t>
-  </si>
-  <si>
-    <t>Facility Internal Undrawn</t>
-  </si>
-  <si>
-    <t>Primary_Lender</t>
-  </si>
-  <si>
-    <t>Primary_LenderLoc</t>
-  </si>
-  <si>
-    <t>Primary_RiskBook</t>
-  </si>
-  <si>
-    <t>Primary_PctOfDeal</t>
-  </si>
-  <si>
-    <t>BuySellPrice</t>
-  </si>
-  <si>
-    <t>SellAmount</t>
-  </si>
-  <si>
-    <t>Primary_Contact</t>
-  </si>
-  <si>
-    <t>Primary_Portfolio</t>
-  </si>
-  <si>
-    <t>Primary_PortfolioBranch</t>
-  </si>
-  <si>
-    <t>Structured Asset Finance</t>
-  </si>
-  <si>
-    <t>02-Jun-2020</t>
-  </si>
-  <si>
-    <t>Facility_Spread</t>
-  </si>
-  <si>
-    <t>Facility_CurrentAvailToDraw</t>
-  </si>
-  <si>
-    <t>Facility_CurrentGlobalOutstandings</t>
-  </si>
-  <si>
-    <t>Outstanding_Type</t>
-  </si>
-  <si>
-    <t>Loan_FacilityName</t>
-  </si>
-  <si>
-    <t>Loan_Alias</t>
-  </si>
-  <si>
-    <t>Loan_PricingOption</t>
-  </si>
-  <si>
-    <t>Loan_RequestedAmount</t>
-  </si>
-  <si>
-    <t>HostBankSharePct</t>
-  </si>
-  <si>
-    <t>Loan_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Loan_MaturityDate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingFrequency</t>
-  </si>
-  <si>
-    <t>Loan_IntCycleFrequency</t>
-  </si>
-  <si>
-    <t>Loan_Accrue</t>
-  </si>
-  <si>
-    <t>Borrower_BaseRate</t>
-  </si>
-  <si>
-    <t>Repayment_ScheduleFrequency</t>
-  </si>
-  <si>
-    <t>Repayment_NumberOfCycles</t>
-  </si>
-  <si>
-    <t>Repayment_TriggerDate</t>
-  </si>
-  <si>
-    <t>Repayment_NonBusDayRule</t>
-  </si>
-  <si>
-    <t>WIP_TransactionType</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingApprovalStatus</t>
-  </si>
-  <si>
-    <t>WIP_OutstandingType</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingRateApprovalStatus</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingReleaseCashflowsStatus</t>
-  </si>
-  <si>
-    <t>Borrower_Profile</t>
-  </si>
-  <si>
-    <t>Remittance_Status</t>
-  </si>
-  <si>
-    <t>Loan_Currency</t>
-  </si>
-  <si>
-    <t>HostBank_GLAccount</t>
-  </si>
-  <si>
-    <t>Borrower_GLAccount</t>
-  </si>
-  <si>
-    <t>Host_Bank</t>
-  </si>
-  <si>
-    <t>NoticeStatus</t>
-  </si>
-  <si>
-    <t>BranchCode</t>
   </si>
   <si>
     <t>0.00</t>
@@ -4060,8 +4060,8 @@
   </sheetPr>
   <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR1" sqref="AR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4130,82 +4130,82 @@
         <v>421</v>
       </c>
       <c r="G1" s="29" t="s">
+        <v>691</v>
+      </c>
+      <c r="H1" s="97" t="s">
         <v>692</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="I1" s="97" t="s">
         <v>693</v>
-      </c>
-      <c r="I1" s="97" t="s">
-        <v>694</v>
       </c>
       <c r="J1" s="30" t="s">
         <v>426</v>
       </c>
       <c r="K1" s="29" t="s">
+        <v>694</v>
+      </c>
+      <c r="L1" s="30" t="s">
         <v>695</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="M1" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="N1" s="29" t="s">
         <v>697</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="O1" s="29" t="s">
         <v>698</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="P1" s="29" t="s">
         <v>699</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="Q1" s="30" t="s">
         <v>700</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="R1" s="30" t="s">
         <v>701</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="S1" s="29" t="s">
         <v>702</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="T1" s="29" t="s">
         <v>703</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="U1" s="29" t="s">
         <v>704</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="V1" s="29" t="s">
         <v>705</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="W1" s="95" t="s">
         <v>706</v>
       </c>
-      <c r="W1" s="95" t="s">
+      <c r="X1" s="95" t="s">
         <v>707</v>
       </c>
-      <c r="X1" s="95" t="s">
+      <c r="Y1" s="30" t="s">
         <v>708</v>
       </c>
-      <c r="Y1" s="30" t="s">
+      <c r="Z1" s="29" t="s">
         <v>709</v>
       </c>
-      <c r="Z1" s="29" t="s">
+      <c r="AA1" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>715</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>716</v>
       </c>
       <c r="AG1" s="13" t="s">
         <v>174</v>
@@ -4217,28 +4217,28 @@
         <v>166</v>
       </c>
       <c r="AJ1" s="94" t="s">
+        <v>716</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>718</v>
       </c>
       <c r="AL1" s="13" t="s">
         <v>588</v>
       </c>
       <c r="AM1" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>722</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>723</v>
       </c>
       <c r="AR1" s="2" t="s">
         <v>295</v>
@@ -4264,7 +4264,7 @@
         <v>517</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>676</v>
+        <v>723</v>
       </c>
       <c r="H2" s="93" t="s">
         <v>638</v>
@@ -4398,7 +4398,7 @@
         <v>551</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>676</v>
+        <v>723</v>
       </c>
       <c r="H3" t="s">
         <v>646</v>
@@ -4563,8 +4563,8 @@
     <col min="14" max="14" width="23.42578125" style="92" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="32.7109375" style="92" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.28515625" style="92" bestFit="1" customWidth="1"/>
-    <col min="17" max="38" width="8.7109375" style="92" customWidth="1"/>
-    <col min="39" max="16384" width="8.7109375" style="92"/>
+    <col min="17" max="39" width="8.7109375" style="92" customWidth="1"/>
+    <col min="40" max="16384" width="8.7109375" style="92"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="87" customFormat="1" x14ac:dyDescent="0.2">
@@ -4893,7 +4893,7 @@
         <v>670</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>676</v>
+        <v>723</v>
       </c>
       <c r="O2" s="20" t="s">
         <v>799</v>
@@ -4959,7 +4959,7 @@
         <v>674</v>
       </c>
       <c r="AJ2" s="22" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AK2" s="93" t="s">
         <v>799</v>
@@ -5193,7 +5193,7 @@
         <v>825</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>826</v>
@@ -5202,19 +5202,19 @@
         <v>166</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>827</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>176</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>828</v>
@@ -5223,16 +5223,16 @@
         <v>829</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>830</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="W1" s="13" t="s">
         <v>831</v>
@@ -5250,10 +5250,10 @@
         <v>227</v>
       </c>
       <c r="AB1" s="13" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="AX1" s="36"/>
       <c r="AY1" s="36"/>
@@ -5496,10 +5496,10 @@
         <v>844</v>
       </c>
       <c r="I1" s="39" t="s">
+        <v>696</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>697</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>698</v>
       </c>
       <c r="K1" s="26" t="s">
         <v>845</v>
@@ -5556,22 +5556,22 @@
         <v>859</v>
       </c>
       <c r="AC1" s="26" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="AD1" s="26" t="s">
+        <v>710</v>
+      </c>
+      <c r="AE1" s="26" t="s">
         <v>711</v>
-      </c>
-      <c r="AE1" s="26" t="s">
-        <v>712</v>
       </c>
       <c r="AF1" s="26" t="s">
         <v>860</v>
       </c>
       <c r="AG1" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="AH1" s="26" t="s">
         <v>715</v>
-      </c>
-      <c r="AH1" s="26" t="s">
-        <v>716</v>
       </c>
       <c r="AI1" s="25" t="s">
         <v>176</v>
@@ -5580,10 +5580,10 @@
         <v>166</v>
       </c>
       <c r="AK1" s="26" t="s">
+        <v>716</v>
+      </c>
+      <c r="AL1" s="26" t="s">
         <v>717</v>
-      </c>
-      <c r="AL1" s="26" t="s">
-        <v>718</v>
       </c>
       <c r="AM1" s="25" t="s">
         <v>166</v>
@@ -5598,16 +5598,16 @@
         <v>862</v>
       </c>
       <c r="AQ1" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="AR1" s="25" t="s">
         <v>719</v>
       </c>
-      <c r="AR1" s="25" t="s">
+      <c r="AS1" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="AT1" s="25" t="s">
         <v>720</v>
-      </c>
-      <c r="AS1" s="25" t="s">
-        <v>700</v>
-      </c>
-      <c r="AT1" s="25" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:46" s="93" customFormat="1" x14ac:dyDescent="0.25">
@@ -5843,28 +5843,28 @@
         <v>826</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>882</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>426</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>176</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="R1" s="34" t="s">
         <v>421</v>
@@ -5900,7 +5900,7 @@
         <v>889</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="AD1" s="2" t="s">
         <v>773</v>
@@ -5927,7 +5927,7 @@
         <v>893</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:38" s="93" customFormat="1" x14ac:dyDescent="0.2">
@@ -6141,8 +6141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6321,10 +6321,10 @@
   <dimension ref="A1:AS8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomRight" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6366,8 +6366,8 @@
     <col min="42" max="42" width="8.7109375" style="64" customWidth="1"/>
     <col min="43" max="43" width="11.28515625" style="64" customWidth="1"/>
     <col min="44" max="45" width="8.7109375" style="64" customWidth="1"/>
-    <col min="46" max="86" width="9.140625" style="68" customWidth="1"/>
-    <col min="87" max="16384" width="9.140625" style="68"/>
+    <col min="46" max="87" width="9.140625" style="68" customWidth="1"/>
+    <col min="88" max="16384" width="9.140625" style="68"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6677,8 +6677,8 @@
   </sheetPr>
   <dimension ref="A1:EI3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="EB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="EH1" sqref="EH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9266,8 +9266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AV6" sqref="AV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9471,7 +9471,9 @@
       <c r="AW1" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="AX1" s="102"/>
+      <c r="AX1" s="102" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="2" spans="1:50" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="93" t="s">
@@ -9617,6 +9619,9 @@
       </c>
       <c r="AW2" s="93" t="s">
         <v>300</v>
+      </c>
+      <c r="AX2" s="93" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -10035,10 +10040,10 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10187,10 +10192,10 @@
         <v>675</v>
       </c>
       <c r="T2" s="93" t="s">
+        <v>676</v>
+      </c>
+      <c r="U2" s="93" t="s">
         <v>677</v>
-      </c>
-      <c r="U2" s="93" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.2">
@@ -10198,7 +10203,7 @@
         <v>394</v>
       </c>
       <c r="B3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C3" t="s">
         <v>551</v>
@@ -10252,10 +10257,10 @@
         <v>675</v>
       </c>
       <c r="T3" s="93" t="s">
+        <v>676</v>
+      </c>
+      <c r="U3" s="93" t="s">
         <v>677</v>
-      </c>
-      <c r="U3" s="93" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.2">
@@ -10263,7 +10268,7 @@
         <v>553</v>
       </c>
       <c r="B4" s="93" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C4" t="s">
         <v>554</v>
@@ -10317,10 +10322,10 @@
         <v>675</v>
       </c>
       <c r="T4" s="93" t="s">
+        <v>676</v>
+      </c>
+      <c r="U4" s="93" t="s">
         <v>677</v>
-      </c>
-      <c r="U4" s="93" t="s">
-        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -10337,9 +10342,9 @@
   </sheetPr>
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W26" sqref="W26"/>
+      <selection pane="topRight" activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10388,13 +10393,13 @@
         <v>421</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>682</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>683</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>198</v>
@@ -10403,28 +10408,28 @@
         <v>507</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>685</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>686</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>565</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>567</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>688</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>689</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>570</v>
@@ -10486,7 +10491,7 @@
         <v>528</v>
       </c>
       <c r="H2" s="93" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I2" s="93" t="s">
         <v>591</v>
@@ -10572,7 +10577,7 @@
         <v>528</v>
       </c>
       <c r="H3" s="93" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I3" s="93" t="s">
         <v>591</v>
@@ -10620,10 +10625,10 @@
         <v>597</v>
       </c>
       <c r="Y3" s="93" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="Z3" s="93" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="AA3" s="93" t="s">
         <v>522</v>
@@ -10658,7 +10663,7 @@
         <v>528</v>
       </c>
       <c r="H4" s="93" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I4" s="93" t="s">
         <v>591</v>
@@ -10706,10 +10711,10 @@
         <v>597</v>
       </c>
       <c r="Y4" s="93" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="Z4" s="93" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="AA4" s="93" t="s">
         <v>522</v>

</xml_diff>

<commit_message>
Feature/GDE-7589 updated source keywords to be reusable
Updated Business process keywords for internal and external
participation
Deleted FACILITY_COUNT global variable on keywords, test suites and
configurations
Update data set
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S2_EU_RPA_ExternallDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S2_EU_RPA_ExternallDeal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2805" yWindow="3375" windowWidth="21600" windowHeight="11385" tabRatio="877" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="5" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SYND02_PrimaryAllocation" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO12_PortfolioSettledDisc" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_InternalParticipation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_ExternalParticipation" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV08_ComprehensiveRepricing" sheetId="13" state="visible" r:id="rId13"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="15" state="visible" r:id="rId15"/>
@@ -2223,8 +2223,8 @@
     <col width="23.42578125" bestFit="1" customWidth="1" style="89" min="14" max="14"/>
     <col width="32.7109375" bestFit="1" customWidth="1" style="89" min="15" max="15"/>
     <col width="12.28515625" bestFit="1" customWidth="1" style="89" min="16" max="16"/>
-    <col width="8.7109375" customWidth="1" style="89" min="17" max="49"/>
-    <col width="8.7109375" customWidth="1" style="89" min="50" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="89" min="17" max="52"/>
+    <col width="8.7109375" customWidth="1" style="89" min="53" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="84">
@@ -2402,10 +2402,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2421,18 +2421,17 @@
     <col width="30.5703125" bestFit="1" customWidth="1" style="117" min="9" max="9"/>
     <col width="31" bestFit="1" customWidth="1" style="117" min="10" max="10"/>
     <col width="11.28515625" bestFit="1" customWidth="1" style="117" min="11" max="11"/>
-    <col width="22.140625" bestFit="1" customWidth="1" style="117" min="12" max="12"/>
-    <col width="26.42578125" customWidth="1" style="117" min="13" max="14"/>
-    <col width="14.42578125" bestFit="1" customWidth="1" style="117" min="15" max="15"/>
-    <col width="19.28515625" bestFit="1" customWidth="1" style="117" min="16" max="16"/>
-    <col width="14.28515625" bestFit="1" customWidth="1" style="117" min="17" max="17"/>
-    <col width="15.28515625" bestFit="1" customWidth="1" style="117" min="18" max="18"/>
-    <col width="37.140625" bestFit="1" customWidth="1" style="117" min="19" max="19"/>
-    <col width="29" bestFit="1" customWidth="1" style="117" min="20" max="20"/>
-    <col width="26.42578125" bestFit="1" customWidth="1" style="117" min="21" max="21"/>
-    <col width="20.7109375" bestFit="1" customWidth="1" style="117" min="22" max="22"/>
-    <col width="35" bestFit="1" customWidth="1" style="117" min="23" max="23"/>
-    <col width="25.140625" bestFit="1" customWidth="1" style="117" min="24" max="24"/>
+    <col width="26.42578125" customWidth="1" style="117" min="12" max="13"/>
+    <col width="14.42578125" bestFit="1" customWidth="1" style="117" min="14" max="14"/>
+    <col width="19.28515625" bestFit="1" customWidth="1" style="117" min="15" max="15"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" style="117" min="16" max="16"/>
+    <col width="15.28515625" bestFit="1" customWidth="1" style="117" min="17" max="17"/>
+    <col width="37.140625" bestFit="1" customWidth="1" style="117" min="18" max="18"/>
+    <col width="29" bestFit="1" customWidth="1" style="117" min="19" max="19"/>
+    <col width="26.42578125" bestFit="1" customWidth="1" style="117" min="20" max="20"/>
+    <col width="20.7109375" bestFit="1" customWidth="1" style="117" min="21" max="21"/>
+    <col width="35" bestFit="1" customWidth="1" style="117" min="22" max="22"/>
+    <col width="25.140625" bestFit="1" customWidth="1" style="117" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" s="117">
@@ -2491,67 +2490,62 @@
           <t>Pct_of_Deal</t>
         </is>
       </c>
-      <c r="L1" s="85" t="inlineStr">
-        <is>
-          <t>Participation_Discount</t>
-        </is>
-      </c>
-      <c r="M1" s="83" t="inlineStr">
+      <c r="L1" s="83" t="inlineStr">
         <is>
           <t>Int_Fee</t>
         </is>
       </c>
-      <c r="N1" s="85" t="inlineStr">
+      <c r="M1" s="85" t="inlineStr">
         <is>
           <t>Buy_Sell_Amount</t>
         </is>
       </c>
-      <c r="O1" s="83" t="inlineStr">
+      <c r="N1" s="83" t="inlineStr">
         <is>
           <t>Buy_Sell_Price</t>
         </is>
       </c>
-      <c r="P1" s="85" t="inlineStr">
+      <c r="O1" s="85" t="inlineStr">
         <is>
           <t>Expected_CloseDate</t>
         </is>
       </c>
+      <c r="P1" s="83" t="inlineStr">
+        <is>
+          <t>Buyer_Contact</t>
+        </is>
+      </c>
       <c r="Q1" s="83" t="inlineStr">
         <is>
-          <t>Buyer_Contact</t>
+          <t>Seller_Contact</t>
         </is>
       </c>
       <c r="R1" s="83" t="inlineStr">
         <is>
-          <t>Seller_Contact</t>
-        </is>
-      </c>
-      <c r="S1" s="83" t="inlineStr">
-        <is>
           <t>Transaction_Status_Awaiting_Approval</t>
         </is>
       </c>
+      <c r="S1" s="84" t="inlineStr">
+        <is>
+          <t>Participation_Transaction_Type</t>
+        </is>
+      </c>
       <c r="T1" s="84" t="inlineStr">
         <is>
-          <t>Participation_Transaction_Type</t>
-        </is>
-      </c>
-      <c r="U1" s="84" t="inlineStr">
-        <is>
           <t>Buyer_Portfolio</t>
         </is>
       </c>
+      <c r="U1" s="83" t="inlineStr">
+        <is>
+          <t>Buyer_ExpenseCode</t>
+        </is>
+      </c>
       <c r="V1" s="83" t="inlineStr">
         <is>
-          <t>Buyer_ExpenseCode</t>
+          <t>Buyer_Branch</t>
         </is>
       </c>
       <c r="W1" s="83" t="inlineStr">
-        <is>
-          <t>Buyer_Branch</t>
-        </is>
-      </c>
-      <c r="X1" s="83" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
@@ -2609,61 +2603,56 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>-250000.0</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
           <t>Actual\Settlement Date</t>
         </is>
       </c>
+      <c r="M2" t="n">
+        <v>50000000</v>
+      </c>
       <c r="N2" t="n">
-        <v>50000000</v>
-      </c>
-      <c r="O2" t="n">
         <v>101</v>
       </c>
-      <c r="P2" s="90" t="inlineStr">
+      <c r="O2" s="90" t="inlineStr">
         <is>
           <t>04-Nov-2020</t>
         </is>
       </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Lending,  Ops</t>
+        </is>
+      </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Lending,  Ops</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
           <t>Loan,  Operations</t>
         </is>
       </c>
-      <c r="S2" s="87" t="inlineStr">
+      <c r="R2" s="87" t="inlineStr">
         <is>
           <t>Awaiting Complete Portfolio Allocations</t>
         </is>
       </c>
+      <c r="S2" s="89" t="inlineStr">
+        <is>
+          <t>Circles</t>
+        </is>
+      </c>
       <c r="T2" s="89" t="inlineStr">
         <is>
-          <t>Circles</t>
-        </is>
-      </c>
-      <c r="U2" s="89" t="inlineStr">
-        <is>
           <t>Hold for Investment - Australia</t>
         </is>
       </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>DM_CFS</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>DM_CFS</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
           <t>Commonwealth Bank of Australia - OBU</t>
         </is>
       </c>
-      <c r="X2" s="111" t="inlineStr">
+      <c r="W2" s="111" t="inlineStr">
         <is>
           <t>IMT</t>
         </is>
@@ -2685,11 +2674,6 @@
           <t>PARDRAW10112020074952SSR</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>-150000.0</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="45" t="inlineStr">
@@ -2705,11 +2689,6 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>INTUND10112020092733NPK</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>-100000.0</t>
         </is>
       </c>
     </row>
@@ -5372,8 +5351,8 @@
     <col width="8.7109375" customWidth="1" style="63" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="63" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="63" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="67" min="46" max="97"/>
-    <col width="9.140625" customWidth="1" style="67" min="98" max="16384"/>
+    <col width="9.140625" customWidth="1" style="67" min="46" max="100"/>
+    <col width="9.140625" customWidth="1" style="67" min="101" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="60">
@@ -10461,7 +10440,7 @@
   </sheetPr>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>

</xml_diff>